<commit_message>
README.md updated for Flight Airspace use case
</commit_message>
<xml_diff>
--- a/src/test/resources/techtest/Aerospace Usecase.xlsx
+++ b/src/test/resources/techtest/Aerospace Usecase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kfplc-my.sharepoint.com/personal/tuhin_chandra_kingfisher_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{8EDC9F36-B5BC-4580-9723-9BB0DC6DC713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEF6ABF9-2D7A-47BC-9C5B-5CD755BB128F}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{8EDC9F36-B5BC-4580-9723-9BB0DC6DC713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ED4DBB6-0922-4DF3-9A00-6F1BE9FAA6CF}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{ACF3ADAA-3380-47C4-984C-DA0E663439D5}"/>
   </bookViews>
@@ -78,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +115,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -143,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -151,6 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,6 +173,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA8A56A-ED0E-4C9D-B6BA-2470047518E3}">
   <dimension ref="G15:NC195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FE38" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="KY69" sqref="KY69"/>
+    <sheetView tabSelected="1" topLeftCell="GC54" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="GC75" sqref="A75:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1918,7 +1929,7 @@
       <c r="HY75" s="5"/>
       <c r="HZ75" s="5"/>
       <c r="IA75" s="5"/>
-      <c r="IB75" s="5"/>
+      <c r="IB75" s="7"/>
       <c r="IC75" s="5"/>
       <c r="ID75" s="5"/>
       <c r="IE75" s="5"/>
@@ -4251,6 +4262,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5226087a-ac3f-461b-b4a3-375f29f6e14a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E72CE0F2B2EC2642BE8BAC0FF81F0123" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2981db008762229a747b36012870b4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5226087a-ac3f-461b-b4a3-375f29f6e14a" xmlns:ns4="bd950485-8efc-4a91-a08d-ecbfc5378e7e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19218db49b00b6025c8404eb87e7e299" ns3:_="" ns4:_="">
     <xsd:import namespace="5226087a-ac3f-461b-b4a3-375f29f6e14a"/>
@@ -4485,24 +4513,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AE91BE4-A656-4F53-B2C2-5934004AD0D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5226087a-ac3f-461b-b4a3-375f29f6e14a"/>
+    <ds:schemaRef ds:uri="bd950485-8efc-4a91-a08d-ecbfc5378e7e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5226087a-ac3f-461b-b4a3-375f29f6e14a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EC886D4-9665-41AE-8467-A145A81A0430}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3563C31C-FA52-48CF-BBB4-ED17783BFCDD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4519,29 +4555,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EC886D4-9665-41AE-8467-A145A81A0430}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AE91BE4-A656-4F53-B2C2-5934004AD0D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5226087a-ac3f-461b-b4a3-375f29f6e14a"/>
-    <ds:schemaRef ds:uri="bd950485-8efc-4a91-a08d-ecbfc5378e7e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>